<commit_message>
fix skippable checking so it actually works, and fix parsing bug for UpgradeShip trigger
</commit_message>
<xml_diff>
--- a/Assets/Resources/mainquestline-kd.xlsx
+++ b/Assets/Resources/mainquestline-kd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sailingwiththegods\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC9E109-736B-40A4-A44A-6081BFC6BF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018F684F-0BE3-41BB-AED6-E008DAB1F66A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="211">
   <si>
     <t>record_id</t>
   </si>
@@ -659,6 +659,9 @@
   </si>
   <si>
     <t>41.207637_29.117577</t>
+  </si>
+  <si>
+    <t>UpgradeShip</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1152,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1216,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
refer to resource name instead of jpg extension in spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Resources/mainquestline-kd.xlsx
+++ b/Assets/Resources/mainquestline-kd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sailingwiththegods\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018F684F-0BE3-41BB-AED6-E008DAB1F66A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B306E49A-A7C1-407E-BF59-B61A92C24EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>You are at Pagasae: you make a big impression! You’re good looking and your ship is (literally) divine: Athena made it, and put in an oracular piece of timber from Dodona, where the gods spoke through the winds in the leaves. Better make the gods happy: you make a sacrifice, have a feast, and sing as song as you set off, led by Orpheus who could sing magical tunes. Herakles was voted captain, but he declined: who could do this better than you? Look in your captain’s log for directions to your next stop.</t>
   </si>
   <si>
-    <t>stop_1.jpg</t>
-  </si>
-  <si>
     <t>“Argonautica / ex conitubis geographicis Abrah. Ortelij (detail)” / Source gallica.bnf.fr / Bibliothèque nationale de France</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>386_319_366</t>
   </si>
   <si>
-    <t>stop_2.jpg</t>
-  </si>
-  <si>
     <t>“Intaglio with a Scene of Sacrifice” / Source © Michael C. Carlos Museum, Emory University. Photo by Bruce M. White, 2005.</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>310_168_152</t>
   </si>
   <si>
-    <t>stop_3.jpg</t>
-  </si>
-  <si>
     <t>“Adieux de Jason à Hypsipyle (Epîtres d’Ovide, Octavien de Saint Gelais)” / Source gallica.bnf.fr / Bibliothèque nationale de France</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>You have arrived at Samothrace: people from all around the Mediterranean came here to be initiated into the secret rites of the Great Gods of the island, for a modest fee which you may also pay! Once initiated you will have the protection of the gods for your ship, and a network of friends from the Black Sea to the delta of Egypt; you may return to observe the island’s festivals, where the history of the island was told in drama and dance.</t>
   </si>
   <si>
-    <t>stop_4.jpg</t>
-  </si>
-  <si>
     <t>“Carola delle Muse.” Epigraphical and archaeological collections including copies of drawings by Ciriaco d'Ancona ('Codex Ashmolensis'). Bartolomeo Fonzio. 15th century, end. / Source Bodleian Library MS. Lat. misc. d. 85. Photo: Bodleian Libraries, University of Oxford 2019.</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
     <t>382_47_235</t>
   </si>
   <si>
-    <t>stop_default.jpg</t>
-  </si>
-  <si>
     <t>“The Argonauts landing at the Tomb of Dolops” / Source Ye gods and little fishes, 1900. Archive.org</t>
   </si>
   <si>
@@ -214,15 +199,9 @@
     <t>14_11_27</t>
   </si>
   <si>
-    <t>stop_6.jpg</t>
-  </si>
-  <si>
     <t>“Hylas and the Nymphs” by John William Waterhouse 1896</t>
   </si>
   <si>
-    <t>https://commons.wikimedia.org/wiki/File:Waterhouse_Hylas_and_the_Nymphs_Manchester_Art_Gallery_1896.15.jpg</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -235,9 +214,6 @@
     <t>You have arrived at Bebrycia – dangers await! King Amycus has a violent streak: he kills foreigners, either by sacrificing them to Poseidon or beating them to death in a boxing match. He cheats: he inserts weighted, spiked metal bits into the leather he uses to wrap his hands, called himantes. Thankfully you have Polydeukes, the great Greek boxer on board, so Amycus meets his bloody match. After Polydeukes kills the king in the boxing ring, you and all your crew get into a battle with his people, - you win with no losses, hold a big feast and set sail for Thynia.</t>
   </si>
   <si>
-    <t>stop_7.jpg</t>
-  </si>
-  <si>
     <t>“Boxers” in Hieronymi Mercvrialis De arte gymnastica libri sex by Girolamo Mercuriale / Source archive.org contributor Getty Resesarch Institute</t>
   </si>
   <si>
@@ -256,9 +232,6 @@
     <t>You have arrived at Hieron, a vital site in Thynia. In historical times, this was the place to celebrate Zeus of the Winds; for the Argonauts, you need to beware the Harpies, the hounds of Zeus! They are women, they are wind, they are violent and they are half-birds. And, they are hungry. And, they smell awful. They punish Phineus, a seer who angered Zeus by giving prophecies that were too accurate; the Harpies snatch his food from his table and befoul what they cannot take. You free the sad old man with the help of Zetes and Calais, two sons of the North Wind who are among your crew: they engage in the first airborne battle in history, driving the Harpies far, far away to the Floating Islands, which were imagined to be in Crete, Sicily or beyond. Here they lock the windy birdwomen underground, and return to their rejoicing buddies. Phineus tells everyone how to get to the Black Sea: you must pass through the clashing rocks. To do this, release a trembling dove and see if she makes it; if the dove survives the rocks, you should follow! If not, go back.</t>
   </si>
   <si>
-    <t>stop_8.jpg</t>
-  </si>
-  <si>
     <t>“The Harpies Driven from the Table of King Phineus by Zetes and Calais” by Francois Verdier / Source The Metropolitan Museum of Art CC-PA</t>
   </si>
   <si>
@@ -277,9 +250,6 @@
     <t>342_256</t>
   </si>
   <si>
-    <t>stop_9.jpg</t>
-  </si>
-  <si>
     <t>“The Argonauts at the Clashing Rocks” in folio g1v: beginning of book 4 (detail) from the Argonautica printed in 1519 by Josse Bade in Paris / Source University of Glasgow Library</t>
   </si>
   <si>
@@ -295,9 +265,6 @@
     <t>You have arrived at Thynias! This is a dry and unpromising desert island but Apollo himself appears to you, riding his chariot across the sky. He is the god who best knows how to bring Greeks to places they had never been. Celebrate him! You build him an altar, celebrating him as Lord of the Dawn; your men dance, pour libations and sing. You spend three days celebrating, and then sail to the Cape of Acherusias.</t>
   </si>
   <si>
-    <t>stop_10.jpg</t>
-  </si>
-  <si>
     <t>“Table top depicting Aurora and the Chariot of Apollo” 1822 by Gioacchino Barberi / Source The Metropolitan Museum of Art CC-PA</t>
   </si>
   <si>
@@ -316,15 +283,9 @@
     <t>16_29</t>
   </si>
   <si>
-    <t>stop_11.jpg</t>
-  </si>
-  <si>
     <t>“Vessel in the Shape of a Wild Boar” from the Cleveland Museum of Art / Source Wikimedia CC0 1.0</t>
   </si>
   <si>
-    <t>https://commons.wikimedia.org/wiki/File:Clevelandart_1977.42.jpg</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -334,9 +295,6 @@
     <t>You have reached Lyra! And once again an ancient hero rises from the tomb to demand attention from you: he cannot stay underground, given the chance to gaze on you (you remind him so much of, well, himself…..). This is Sthenelaos, who was killed while accompanying Herakles on his quest to steal the belt of the Amazon queen. That belt is a metaphor for all her power – and Sthenelaos lost all of his, meeting his doom in the quest. Herakles himself built the tomb for his friend; Mopsos the seer tells you to approach the tomb, offer Sthenelaos some libations, and build an altar to Apollo who Saves our Ships. Orpheus offered his lyre as a gift to the god, and the name ‘Lyre’ to the place he left it. The next morning you head out for Sinope.</t>
   </si>
   <si>
-    <t>stop_12.jpg</t>
-  </si>
-  <si>
     <t>“Column-Krater Depicting Orpheus among the Thracians” from the Carlos Museum / Source © Michael C. Carlos Museum, Emory Unversity. Photo by Bruce M. White 2010.</t>
   </si>
   <si>
@@ -358,9 +316,6 @@
     <t>34_35_36</t>
   </si>
   <si>
-    <t>stop_13.jpg</t>
-  </si>
-  <si>
     <t>“Sinope” from A voyage into the Levant, vol. 2 by Joseph Pitton de Tournefort 1718 / Source archive.org contributor Getty Research Institute</t>
   </si>
   <si>
@@ -376,15 +331,9 @@
     <t>You have arrived at the icy cold Thermodon River. The Amazons dwell here: they are powerful women who have no fondness for the Greeks! Some say they descended from the Scythians and Sarmatians; others that they were the daughters of Ares, god of war, and the nymph Harmonia. See the image of their city in flames as they battle Theseus’ Athenians (Hdt. 4.110) – happily enough you don’t have to fight them. The winds take you away to Ares’ island before you meet them.</t>
   </si>
   <si>
-    <t>stop_14.jpg</t>
-  </si>
-  <si>
     <t>“The Battle of the Amazons” by Peter Paul Rubens circa 1619 / Source Wikimedia Public Domain</t>
   </si>
   <si>
-    <t>https://commons.wikimedia.org/wiki/File:Peter_Paul_Rubens_007.jpg</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -394,9 +343,6 @@
     <t>You have come to the island of Ares – here the Amazons worship the war god who may be their father, but certainly is as deadly as can be. Even the birds are scary here. They shoot feathers like arrows! Shooting back is useful, but you and your men frighten them by clanging your spears and shields together: they can’t stand the racket and fly away. Here you meet the sons of Phrixus. Phrixus, when just a little boy, was to be sacrificed along with his sister Helle, because of the machinations of his evil stepmother Ino. Their mother Nephele, a cloud nymph, wouldn’t let this happen, and sent a flying golden ram to save them. Helle fell off and drowned in the waters now called the Hellespont; Phrixus made it all the way to Colchis where he sacrificed the ram to Zeus, settled down, got married, and had some baby heroes. Its fleece is now your goal!</t>
   </si>
   <si>
-    <t>stop_15.jpg</t>
-  </si>
-  <si>
     <t>“The Legend of Phrixus and Helles” by Dylazuna / Source Deviant Art, image copyright Dylazuna all rights reserved</t>
   </si>
   <si>
@@ -415,9 +361,6 @@
     <t>173_123</t>
   </si>
   <si>
-    <t>stop_16.jpg</t>
-  </si>
-  <si>
     <t>“De Medee a Iason (Epîtres d’Ovide, Octavien de Saint Gelais)” Source gallica.bnf.fr / Bibliothèque nationale de France</t>
   </si>
   <si>
@@ -436,15 +379,9 @@
     <t>Medea has ordered you to put in at Paphlagonia, in order to perform rites thanking Hekate for her aid in the quest: you would never have succeeded without her! You follow Medea’s instructions: Hekate is a frightful goddess, and her rites are unspeakable. Next you remember Phineus’ prophecy that you would not sail back the way you came, and you set out for Bryges.</t>
   </si>
   <si>
-    <t>stop_18.jpg</t>
-  </si>
-  <si>
     <t>“Map of Apollonius Rhodius' Argonautica”, reprint of Ortelius' Parergon, 1624 / Source Wikimedia CC-PD</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Argonautica#/media/File:MapoftheVoyageoftheArgonauts.jpg</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -662,6 +599,69 @@
   </si>
   <si>
     <t>UpgradeShip</t>
+  </si>
+  <si>
+    <t>stop_1</t>
+  </si>
+  <si>
+    <t>stop_2</t>
+  </si>
+  <si>
+    <t>stop_3</t>
+  </si>
+  <si>
+    <t>stop_4</t>
+  </si>
+  <si>
+    <t>stop_default</t>
+  </si>
+  <si>
+    <t>stop_6</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Waterhouse_Hylas_and_the_Nymphs_Manchester_Art_Gallery_1896.15</t>
+  </si>
+  <si>
+    <t>stop_7</t>
+  </si>
+  <si>
+    <t>stop_8</t>
+  </si>
+  <si>
+    <t>stop_9</t>
+  </si>
+  <si>
+    <t>stop_10</t>
+  </si>
+  <si>
+    <t>stop_11</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Clevelandart_1977.42</t>
+  </si>
+  <si>
+    <t>stop_12</t>
+  </si>
+  <si>
+    <t>stop_13</t>
+  </si>
+  <si>
+    <t>stop_14</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Peter_Paul_Rubens_007</t>
+  </si>
+  <si>
+    <t>stop_15</t>
+  </si>
+  <si>
+    <t>stop_16</t>
+  </si>
+  <si>
+    <t>stop_18</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Argonautica#/media/File:MapoftheVoyageoftheArgonauts</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1216,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -1228,7 +1228,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>16</v>
@@ -1251,7 +1251,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
@@ -1263,7 +1263,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>21</v>
@@ -1278,103 +1278,103 @@
         <v>-1</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="F5" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1383,136 +1383,136 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="I7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="K8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="M8" s="4" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2">
         <v>227</v>
@@ -1524,36 +1524,36 @@
         <v>-1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H10" s="2">
         <v>162</v>
@@ -1565,39 +1565,39 @@
         <v>-1</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="D11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I11" s="2">
         <v>-1</v>
@@ -1606,21 +1606,21 @@
         <v>-1</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C12" s="5">
         <v>385</v>
@@ -1629,16 +1629,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I12" s="2">
         <v>-1</v>
@@ -1647,21 +1647,21 @@
         <v>-1</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C13" s="5">
         <v>169</v>
@@ -1670,13 +1670,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H13" s="2">
         <v>359</v>
@@ -1685,24 +1685,24 @@
         <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>95</v>
+        <v>201</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>97</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C14" s="5">
         <v>274</v>
@@ -1711,13 +1711,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H14" s="2">
         <v>349</v>
@@ -1729,21 +1729,21 @@
         <v>-1</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C15" s="6">
         <v>445</v>
@@ -1752,39 +1752,39 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="J15" s="2">
         <v>-1</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C16" s="5">
         <v>380</v>
@@ -1793,13 +1793,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H16" s="2">
         <v>350</v>
@@ -1811,21 +1811,21 @@
         <v>-1</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>117</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C17" s="5">
         <v>226</v>
@@ -1834,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="H17" s="2">
         <v>-1</v>
@@ -1852,21 +1852,21 @@
         <v>-1</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>121</v>
+        <v>207</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C18" s="5">
         <v>402</v>
@@ -1875,55 +1875,55 @@
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I18" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="L18" s="2" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="H19" s="2">
         <v>350</v>
@@ -1935,37 +1935,37 @@
         <v>-1</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>137</v>
+        <v>210</v>
       </c>
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="H20" s="2">
         <v>252</v>
@@ -1977,37 +1977,37 @@
         <v>-1</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="H21" s="2">
         <v>218</v>
@@ -2019,37 +2019,37 @@
         <v>-1</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="D22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="H22" s="2">
         <v>-1</v>
@@ -2061,40 +2061,40 @@
         <v>-1</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="I23" s="2">
         <v>-1</v>
@@ -2103,37 +2103,37 @@
         <v>-1</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="D24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="H24" s="2">
         <v>-1</v>
@@ -2145,37 +2145,37 @@
         <v>-1</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="D25" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="H25" s="2">
         <v>-1</v>
@@ -2187,40 +2187,40 @@
         <v>-1</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="I26" s="2">
         <v>-1</v>
@@ -2229,37 +2229,37 @@
         <v>7</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="N26" s="7"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="D27" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="H27" s="2">
         <v>392</v>
@@ -2271,37 +2271,37 @@
         <v>-1</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="H28" s="2">
         <v>-1</v>
@@ -2313,79 +2313,79 @@
         <v>-1</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="D29" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="I29" s="2">
         <v>-1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="N29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="D30" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="H30" s="2">
         <v>237</v>
@@ -2397,37 +2397,37 @@
         <v>-1</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="N30" s="7"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="H31" s="2">
         <v>-1</v>
@@ -2439,13 +2439,13 @@
         <v>-1</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="N31" s="7"/>
     </row>
@@ -2454,7 +2454,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>19</v>
@@ -2463,13 +2463,13 @@
         <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="H32" s="2">
         <v>221</v>
@@ -2481,13 +2481,13 @@
         <v>-1</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
pull objective strings from spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Resources/mainquestline-kd.xlsx
+++ b/Assets/Resources/mainquestline-kd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sailingwiththegods\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B306E49A-A7C1-407E-BF59-B61A92C24EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD92A14A-A9BB-40EA-8BC9-EF2117B65F01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">Sheet2!$A$1:$J$32</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">Sheet2!$A$1:$K$32</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="242">
   <si>
     <t>record_id</t>
   </si>
@@ -662,6 +662,99 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Argonautica#/media/File:MapoftheVoyageoftheArgonauts</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>Find your way to Pagasae</t>
+  </si>
+  <si>
+    <t>Upgrade your ship to the trireme</t>
+  </si>
+  <si>
+    <t>Find your way to the tomb of Dolops</t>
+  </si>
+  <si>
+    <t>Go to Lemnos</t>
+  </si>
+  <si>
+    <t>Find your way to Samothrace</t>
+  </si>
+  <si>
+    <t>Find your way to Cyzicus</t>
+  </si>
+  <si>
+    <t>Find your way to Mysia</t>
+  </si>
+  <si>
+    <t>Make your way to Bebrycia</t>
+  </si>
+  <si>
+    <t>Make your way to Thynias</t>
+  </si>
+  <si>
+    <t>Head to Hieron</t>
+  </si>
+  <si>
+    <t>Continue east to Acherusia</t>
+  </si>
+  <si>
+    <t>Sail to Lyra</t>
+  </si>
+  <si>
+    <t>Look for Sinope</t>
+  </si>
+  <si>
+    <t>Make your way to Thermodon</t>
+  </si>
+  <si>
+    <t>Go to the island of Ares</t>
+  </si>
+  <si>
+    <t>Head to Aea</t>
+  </si>
+  <si>
+    <t>Sail to Paphlagonia</t>
+  </si>
+  <si>
+    <t>Head to Bryges</t>
+  </si>
+  <si>
+    <t>Sail to the island of Electra</t>
+  </si>
+  <si>
+    <t>Find the City of Hyllus</t>
+  </si>
+  <si>
+    <t>Find Circe</t>
+  </si>
+  <si>
+    <t>Find your way to Aethalia</t>
+  </si>
+  <si>
+    <t>Make your way to Aeaea</t>
+  </si>
+  <si>
+    <t>Find your way to Drepane</t>
+  </si>
+  <si>
+    <t>Make a journey to Syrtis</t>
+  </si>
+  <si>
+    <t>Travel to Lake Triton</t>
+  </si>
+  <si>
+    <t>Sail to Crete</t>
+  </si>
+  <si>
+    <t>Head to Anaphe</t>
+  </si>
+  <si>
+    <t>Find a path to Aegina</t>
+  </si>
+  <si>
+    <t>Return to Pagasae</t>
   </si>
 </sst>
 </file>
@@ -749,7 +842,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -831,13 +929,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="main_questline_database" displayName="main_questline_database" ref="A1:M32" totalsRowShown="0">
-  <autoFilter ref="A1:M32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="main_questline_database" displayName="main_questline_database" ref="A1:N32" totalsRowShown="0">
+  <autoFilter ref="A1:N32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="record_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="trigger type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="trigger data"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="skippable"/>
+    <tableColumn id="14" xr3:uid="{6812246E-36D2-4FB9-9FD7-9A7EB59B4404}" name="objective" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="description"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="arrival event type"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="arrival event data"/>
@@ -1149,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,16 +1260,17 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="74.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
-    <col min="11" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="81.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="74.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="12" max="1026" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1184,34 +1284,37 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1224,29 +1327,32 @@
       <c r="D2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2">
-        <v>-1</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2">
+        <v>-1</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1259,35 +1365,38 @@
       <c r="D3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2">
-        <v>-1</v>
-      </c>
       <c r="I3" s="2">
         <v>-1</v>
       </c>
       <c r="J3" s="2">
         <v>-1</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1300,35 +1409,38 @@
       <c r="D4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="2">
-        <v>-1</v>
-      </c>
       <c r="J4" s="2">
         <v>-1</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1341,35 +1453,38 @@
       <c r="D5" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="2">
-        <v>-1</v>
-      </c>
       <c r="J5" s="2">
         <v>-1</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -1382,35 +1497,38 @@
       <c r="D6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
       <c r="I6" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J6" s="2">
         <v>-1</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
@@ -1423,35 +1541,38 @@
       <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="2">
-        <v>-1</v>
-      </c>
       <c r="J7" s="2">
         <v>-1</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1464,35 +1585,38 @@
       <c r="D8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1505,35 +1629,38 @@
       <c r="D9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>227</v>
       </c>
-      <c r="I9" s="2">
-        <v>-1</v>
-      </c>
       <c r="J9" s="2">
         <v>-1</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -1546,35 +1673,38 @@
       <c r="D10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>162</v>
       </c>
-      <c r="I10" s="2">
-        <v>-1</v>
-      </c>
       <c r="J10" s="2">
         <v>-1</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>69</v>
       </c>
@@ -1587,35 +1717,38 @@
       <c r="D11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="2">
-        <v>-1</v>
-      </c>
       <c r="J11" s="2">
         <v>-1</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
@@ -1628,35 +1761,38 @@
       <c r="D12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>186</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="2">
-        <v>-1</v>
-      </c>
       <c r="J12" s="2">
         <v>-1</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>80</v>
       </c>
@@ -1669,35 +1805,38 @@
       <c r="D13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>359</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>30</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
@@ -1710,35 +1849,38 @@
       <c r="D14" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>349</v>
       </c>
-      <c r="I14" s="2">
-        <v>-1</v>
-      </c>
       <c r="J14" s="2">
         <v>-1</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>90</v>
       </c>
@@ -1751,35 +1893,38 @@
       <c r="D15" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
@@ -1792,35 +1937,38 @@
       <c r="D16" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>350</v>
       </c>
-      <c r="I16" s="2">
-        <v>-1</v>
-      </c>
       <c r="J16" s="2">
         <v>-1</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
@@ -1833,35 +1981,38 @@
       <c r="D17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="2">
-        <v>-1</v>
-      </c>
       <c r="I17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="2">
         <v>31</v>
       </c>
-      <c r="J17" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -1874,36 +2025,39 @@
       <c r="D18" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I18" s="2">
-        <v>-1</v>
-      </c>
       <c r="J18" s="2">
         <v>-1</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>112</v>
       </c>
@@ -1916,36 +2070,39 @@
       <c r="D19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>350</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>32</v>
       </c>
-      <c r="J19" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="N19" s="7"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>117</v>
       </c>
@@ -1958,36 +2115,39 @@
       <c r="D20" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>252</v>
       </c>
-      <c r="I20" s="2">
-        <v>-1</v>
-      </c>
       <c r="J20" s="2">
         <v>-1</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N20" s="7"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>121</v>
       </c>
@@ -2000,36 +2160,39 @@
       <c r="D21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>218</v>
       </c>
-      <c r="I21" s="2">
-        <v>-1</v>
-      </c>
       <c r="J21" s="2">
         <v>-1</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
@@ -2042,36 +2205,39 @@
       <c r="D22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="2">
-        <v>-1</v>
-      </c>
       <c r="I22" s="2">
         <v>-1</v>
       </c>
       <c r="J22" s="2">
         <v>-1</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>131</v>
       </c>
@@ -2084,36 +2250,39 @@
       <c r="D23" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I23" s="2">
-        <v>-1</v>
-      </c>
       <c r="J23" s="2">
         <v>-1</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>137</v>
       </c>
@@ -2126,36 +2295,39 @@
       <c r="D24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="2">
-        <v>-1</v>
-      </c>
       <c r="I24" s="2">
         <v>-1</v>
       </c>
       <c r="J24" s="2">
         <v>-1</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="N24" s="7"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>142</v>
       </c>
@@ -2168,36 +2340,39 @@
       <c r="D25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H25" s="2">
-        <v>-1</v>
-      </c>
       <c r="I25" s="2">
         <v>-1</v>
       </c>
       <c r="J25" s="2">
         <v>-1</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="N25" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>147</v>
       </c>
@@ -2210,36 +2385,39 @@
       <c r="D26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I26" s="2">
-        <v>-1</v>
-      </c>
       <c r="J26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K26" s="2">
         <v>7</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>153</v>
       </c>
@@ -2252,36 +2430,39 @@
       <c r="D27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>392</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>33</v>
       </c>
-      <c r="J27" s="2">
-        <v>-1</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>158</v>
       </c>
@@ -2294,36 +2475,39 @@
       <c r="D28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H28" s="2">
-        <v>-1</v>
-      </c>
       <c r="I28" s="2">
         <v>-1</v>
       </c>
       <c r="J28" s="2">
         <v>-1</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>163</v>
       </c>
@@ -2336,36 +2520,39 @@
       <c r="D29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I29" s="2">
-        <v>-1</v>
-      </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="N29" s="7"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>170</v>
       </c>
@@ -2378,36 +2565,39 @@
       <c r="D30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>237</v>
       </c>
-      <c r="I30" s="2">
-        <v>-1</v>
-      </c>
       <c r="J30" s="2">
         <v>-1</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>175</v>
       </c>
@@ -2420,36 +2610,39 @@
       <c r="D31" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H31" s="2">
-        <v>-1</v>
-      </c>
       <c r="I31" s="2">
         <v>-1</v>
       </c>
       <c r="J31" s="2">
         <v>-1</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N31" s="7"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="7"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -2462,36 +2655,39 @@
       <c r="D32" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>221</v>
       </c>
-      <c r="I32" s="2">
-        <v>-1</v>
-      </c>
       <c r="J32" s="2">
         <v>-1</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="9"/>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
quest confirmed working through thynia, made navigator and crew beacons different colors, fixed bug where the tavern ui showed the same price for everything
</commit_message>
<xml_diff>
--- a/Assets/Resources/mainquestline-kd.xlsx
+++ b/Assets/Resources/mainquestline-kd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sailingwiththegods\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD92A14A-A9BB-40EA-8BC9-EF2117B65F01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0AB5DA-5193-4052-9FAE-20E44A07EA6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -694,9 +694,6 @@
     <t>Make your way to Thynias</t>
   </si>
   <si>
-    <t>Head to Hieron</t>
-  </si>
-  <si>
     <t>Continue east to Acherusia</t>
   </si>
   <si>
@@ -755,6 +752,9 @@
   </si>
   <si>
     <t>Return to Pagasae</t>
+  </si>
+  <si>
+    <t>Head to Thynia</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>65</v>
@@ -1806,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>81</v>
@@ -1850,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>86</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>91</v>
@@ -1938,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>98</v>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>102</v>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>107</v>
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>114</v>
@@ -2116,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>119</v>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>123</v>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>128</v>
@@ -2251,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>133</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>139</v>
@@ -2341,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>144</v>
@@ -2386,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>149</v>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>155</v>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>160</v>
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>165</v>
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>172</v>
@@ -2611,7 +2611,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>177</v>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
golden fleece quiz working
</commit_message>
<xml_diff>
--- a/Assets/Resources/mainquestline-kd.xlsx
+++ b/Assets/Resources/mainquestline-kd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sailingwiththegods\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8C4492-58C0-4FC9-A00C-60912F0AC8C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F2D83-D9EF-4E43-9D6D-D9C694AF08A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,12 +706,6 @@
     <t>Make your way to Thermodon</t>
   </si>
   <si>
-    <t>Go to the island of Ares</t>
-  </si>
-  <si>
-    <t>Head to Aea</t>
-  </si>
-  <si>
     <t>Sail to Paphlagonia</t>
   </si>
   <si>
@@ -758,6 +752,12 @@
   </si>
   <si>
     <t>342_256_385</t>
+  </si>
+  <si>
+    <t>Make your way to Giresun</t>
+  </si>
+  <si>
+    <t>Look for the Phasis river!</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>65</v>
@@ -1733,7 +1733,7 @@
         <v>71</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J11" s="2">
         <v>-1</v>
@@ -1985,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>102</v>
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>107</v>
@@ -2074,7 +2074,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>114</v>
@@ -2119,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>119</v>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>123</v>
@@ -2209,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>128</v>
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>133</v>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>139</v>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>144</v>
@@ -2389,7 +2389,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>149</v>
@@ -2434,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>155</v>
@@ -2479,7 +2479,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>160</v>
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>165</v>
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>172</v>
@@ -2614,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>177</v>
@@ -2659,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>180</v>

</xml_diff>